<commit_message>
Se arreglaron errores en varios registros, hora fija y sleep de 22 horas
</commit_message>
<xml_diff>
--- a/app/src/test.xlsx
+++ b/app/src/test.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thomas Esteban\Escritorio\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thomas Esteban\PycharmProjects\revisionDeActuacionesConsola\app\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6EF5388E-C412-4269-977B-DFBF0044D892}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFFBCE9B-12C9-4DAA-BF7D-98CA0AA3C211}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{E08B5D3B-FE20-463B-A2F3-5802FD490429}"/>
   </bookViews>
@@ -36,27 +36,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>NUMERO DE RADICACION</t>
   </si>
   <si>
-    <t>11001310300620180010600</t>
+    <t>11001310300520210054100</t>
   </si>
   <si>
-    <t>11001310300820230003100</t>
-  </si>
-  <si>
-    <t>11001310301920220022300</t>
-  </si>
-  <si>
-    <t>11001310303620170077300</t>
-  </si>
-  <si>
-    <t>11001310302520220049300</t>
-  </si>
-  <si>
-    <t>11001310301920220051200</t>
+    <t>11001310300420170072500</t>
   </si>
 </sst>
 </file>
@@ -72,21 +60,15 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
-        <bgColor theme="4" tint="0.79998168889431442"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -109,33 +91,16 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -470,10 +435,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87272DE3-A10F-41C1-A680-B99E5F4CE702}">
-  <dimension ref="B1:B7"/>
+  <dimension ref="B1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -496,26 +461,6 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B4" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B5" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B6" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B7" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>